<commit_message>
Adding new FDOM and POC data
</commit_message>
<xml_diff>
--- a/01_Raw_data/POC.xlsx
+++ b/01_Raw_data/POC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Howley_Bradford_Streams\Howley_Bradford_Streams\01_Raw_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6429F0-FF73-48EA-AA00-B5DBFE113051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA3466F-BDB8-44DF-A66B-049DE1DF7597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="44">
   <si>
     <t>Sampled</t>
   </si>
@@ -537,25 +537,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099139EA-B059-430C-B410-93782515C830}">
-  <dimension ref="A1:K79"/>
+  <dimension ref="A1:K87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I70" sqref="I70:I79"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O90" sqref="O90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.40625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
-    <col min="5" max="5" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +590,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45353</v>
       </c>
@@ -623,11 +623,11 @@
         <v>11.299999999999866</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K79" si="0">J2/(C2/1000)</f>
+        <f t="shared" ref="K2:K87" si="0">J2/(C2/1000)</f>
         <v>75.838926174495739</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45019</v>
       </c>
@@ -664,7 +664,7 @@
         <v>6.6339066339067223</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45355</v>
       </c>
@@ -693,7 +693,7 @@
         <v>15</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J79" si="1">(F4-H4)*1000</f>
+        <f t="shared" ref="J4:J87" si="1">(F4-H4)*1000</f>
         <v>4.0000000000000036</v>
       </c>
       <c r="K4">
@@ -701,7 +701,7 @@
         <v>7.326007326007332</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45355</v>
       </c>
@@ -738,7 +738,7 @@
         <v>8.1936685288639843</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45376</v>
       </c>
@@ -775,7 +775,7 @@
         <v>9.1726618705033847</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45376</v>
       </c>
@@ -812,7 +812,7 @@
         <v>7.089552238806017</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45397</v>
       </c>
@@ -831,7 +831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45391</v>
       </c>
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45355</v>
       </c>
@@ -887,7 +887,7 @@
         <v>2.2865853658537452</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45397</v>
       </c>
@@ -924,7 +924,7 @@
         <v>12.315270935960601</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45385</v>
       </c>
@@ -961,7 +961,7 @@
         <v>0.87124878993235522</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45391</v>
       </c>
@@ -998,7 +998,7 @@
         <v>13.29949238578669</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45391</v>
       </c>
@@ -1035,7 +1035,7 @@
         <v>29.107142857142826</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45047</v>
       </c>
@@ -1072,7 +1072,7 @@
         <v>71.755725190840266</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45376</v>
       </c>
@@ -1109,7 +1109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45019</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>11.627906976744121</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45376</v>
       </c>
@@ -1183,7 +1183,7 @@
         <v>4.4692737430166805</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45376</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>9.2957746478875514</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44280</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>13.79962192816609</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45400</v>
       </c>
@@ -1294,7 +1294,7 @@
         <v>45.102505694760907</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45400</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>5.525846702317077</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45355</v>
       </c>
@@ -1368,7 +1368,7 @@
         <v>5.9149722735672263</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45355</v>
       </c>
@@ -1405,7 +1405,7 @@
         <v>5.2346570397110153</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45413</v>
       </c>
@@ -1442,7 +1442,7 @@
         <v>12.145748987854711</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45400</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>6.4864864864861715</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45047</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>8.6021505376343566</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45355</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>6.126126126126251</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45355</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>11.460258780036938</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45376</v>
       </c>
@@ -1627,7 +1627,7 @@
         <v>2.752293577981348</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45385</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>10.609037328094443</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45376</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>5.1282051282049697</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45376</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>5.6558363417568316</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45385</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>22.98850574712646</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45047</v>
       </c>
@@ -1812,7 +1812,7 @@
         <v>4.2521994134899188</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45355</v>
       </c>
@@ -1849,7 +1849,7 @@
         <v>4.676258992806039</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45355</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>13.120567375886656</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45385</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>-1000.132625994695</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45355</v>
       </c>
@@ -1960,7 +1960,7 @@
         <v>2.9090909090909922</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45385</v>
       </c>
@@ -1994,7 +1994,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45047</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>34.965034965034221</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45400</v>
       </c>
@@ -2068,7 +2068,7 @@
         <v>5.7142857142855386</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45397</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>74.855491329479236</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45391</v>
       </c>
@@ -2142,7 +2142,7 @@
         <v>23.317865429234349</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45391</v>
       </c>
@@ -2179,7 +2179,7 @@
         <v>3.231939163497954</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45404</v>
       </c>
@@ -2216,7 +2216,7 @@
         <v>10.958904109589238</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45406</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>208.39999999999924</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45025</v>
       </c>
@@ -2290,7 +2290,7 @@
         <v>42.487046632124276</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45038</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>65.972222222221902</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45406</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>15.122873345935741</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45397</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>13.130252100840289</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45397</v>
       </c>
@@ -2438,7 +2438,7 @@
         <v>31.738035264483486</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45397</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>9.7500000000000355</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45420</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>8.04828973843059</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45420</v>
       </c>
@@ -2549,7 +2549,7 @@
         <v>1.6666666666666885</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>45404</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>8.8631984585740611</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>45420</v>
       </c>
@@ -2623,7 +2623,7 @@
         <v>21.448999046711332</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>45404</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>5.7142857142859302</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>45420</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>1.9848771266540555</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>45415</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>1.7985611510789385</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>45404</v>
       </c>
@@ -2771,7 +2771,7 @@
         <v>2.9978586723767813</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>45415</v>
       </c>
@@ -2808,7 +2808,7 @@
         <v>15.845070422535422</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>45413</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>44.265593561368256</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>45415</v>
       </c>
@@ -2882,7 +2882,7 @@
         <v>5.4669703872436397</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>45420</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>2.7571580063626042</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>45413</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>82.442748091604145</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>45413</v>
       </c>
@@ -2993,7 +2993,7 @@
         <v>25.306122448979526</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>45413</v>
       </c>
@@ -3030,7 +3030,7 @@
         <v>21.192052980132324</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>45415</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>5.5555555555558245</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>45484</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>2.6465028355384606</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>45475</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>6.0185185185183698</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>45484</v>
       </c>
@@ -3178,7 +3178,7 @@
         <v>-0.18181818181816178</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>45442</v>
       </c>
@@ -3215,7 +3215,7 @@
         <v>6.1790668348046989</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>45484</v>
       </c>
@@ -3252,7 +3252,7 @@
         <v>-1.2433392539967052</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>45475</v>
       </c>
@@ -3289,7 +3289,7 @@
         <v>7.7562326869809857</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>45442</v>
       </c>
@@ -3326,7 +3326,7 @@
         <v>3.2258064516127654</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>45442</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>1.7733990147783487</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>45484</v>
       </c>
@@ -3400,7 +3400,7 @@
         <v>6.9029850746269332</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>45484</v>
       </c>
@@ -3435,6 +3435,302 @@
       <c r="K79">
         <f t="shared" si="0"/>
         <v>12.226277372262642</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>45505</v>
+      </c>
+      <c r="B80">
+        <v>6.6</v>
+      </c>
+      <c r="C80">
+        <v>565</v>
+      </c>
+      <c r="D80">
+        <v>1.0686</v>
+      </c>
+      <c r="E80" s="3">
+        <v>45509</v>
+      </c>
+      <c r="F80">
+        <v>1.1884999999999999</v>
+      </c>
+      <c r="G80" s="3">
+        <v>45509</v>
+      </c>
+      <c r="H80">
+        <v>1.1814</v>
+      </c>
+      <c r="I80" t="s">
+        <v>43</v>
+      </c>
+      <c r="J80">
+        <f t="shared" si="1"/>
+        <v>7.0999999999998842</v>
+      </c>
+      <c r="K80">
+        <f t="shared" si="0"/>
+        <v>12.566371681415726</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>45502</v>
+      </c>
+      <c r="B81">
+        <v>15</v>
+      </c>
+      <c r="C81">
+        <v>560</v>
+      </c>
+      <c r="D81">
+        <v>1.1224000000000001</v>
+      </c>
+      <c r="E81" s="3">
+        <v>45509</v>
+      </c>
+      <c r="F81">
+        <v>1.2423999999999999</v>
+      </c>
+      <c r="G81" s="3">
+        <v>45509</v>
+      </c>
+      <c r="H81">
+        <v>1.2336</v>
+      </c>
+      <c r="I81" t="s">
+        <v>43</v>
+      </c>
+      <c r="J81">
+        <f t="shared" si="1"/>
+        <v>8.799999999999919</v>
+      </c>
+      <c r="K81">
+        <f t="shared" si="0"/>
+        <v>15.714285714285568</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>45502</v>
+      </c>
+      <c r="B82">
+        <v>9</v>
+      </c>
+      <c r="C82">
+        <v>563</v>
+      </c>
+      <c r="D82">
+        <v>1.1046</v>
+      </c>
+      <c r="E82" s="3">
+        <v>45509</v>
+      </c>
+      <c r="F82">
+        <v>1.2242</v>
+      </c>
+      <c r="G82" s="3">
+        <v>45509</v>
+      </c>
+      <c r="H82">
+        <v>1.2197</v>
+      </c>
+      <c r="I82" t="s">
+        <v>43</v>
+      </c>
+      <c r="J82">
+        <f t="shared" si="1"/>
+        <v>4.4999999999999485</v>
+      </c>
+      <c r="K82">
+        <f t="shared" si="0"/>
+        <v>7.992895204262787</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>45502</v>
+      </c>
+      <c r="B83">
+        <v>6</v>
+      </c>
+      <c r="C83">
+        <v>554</v>
+      </c>
+      <c r="D83">
+        <v>1.1166</v>
+      </c>
+      <c r="E83" s="3">
+        <v>45509</v>
+      </c>
+      <c r="F83">
+        <v>1.2376</v>
+      </c>
+      <c r="G83" s="3">
+        <v>45509</v>
+      </c>
+      <c r="H83">
+        <v>1.2316</v>
+      </c>
+      <c r="I83" t="s">
+        <v>43</v>
+      </c>
+      <c r="J83">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000053</v>
+      </c>
+      <c r="K83">
+        <f t="shared" si="0"/>
+        <v>10.830324909747301</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>45505</v>
+      </c>
+      <c r="B84">
+        <v>5.5</v>
+      </c>
+      <c r="C84">
+        <v>556</v>
+      </c>
+      <c r="D84">
+        <v>1.0638000000000001</v>
+      </c>
+      <c r="E84" s="3">
+        <v>45509</v>
+      </c>
+      <c r="F84">
+        <v>1.1865000000000001</v>
+      </c>
+      <c r="G84" s="3">
+        <v>45509</v>
+      </c>
+      <c r="H84">
+        <v>1.18</v>
+      </c>
+      <c r="I84" t="s">
+        <v>43</v>
+      </c>
+      <c r="J84">
+        <f t="shared" si="1"/>
+        <v>6.5000000000001723</v>
+      </c>
+      <c r="K84">
+        <f t="shared" si="0"/>
+        <v>11.690647482014697</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>45502</v>
+      </c>
+      <c r="B85" t="s">
+        <v>13</v>
+      </c>
+      <c r="C85">
+        <v>563</v>
+      </c>
+      <c r="D85">
+        <v>1.1358999999999999</v>
+      </c>
+      <c r="E85" s="3">
+        <v>45509</v>
+      </c>
+      <c r="F85">
+        <v>1.2545999999999999</v>
+      </c>
+      <c r="G85" s="3">
+        <v>45509</v>
+      </c>
+      <c r="H85">
+        <v>1.2507999999999999</v>
+      </c>
+      <c r="I85" t="s">
+        <v>43</v>
+      </c>
+      <c r="J85">
+        <f t="shared" si="1"/>
+        <v>3.8000000000000256</v>
+      </c>
+      <c r="K85">
+        <f t="shared" si="0"/>
+        <v>6.7495559502664761</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>45502</v>
+      </c>
+      <c r="B86">
+        <v>5</v>
+      </c>
+      <c r="C86">
+        <v>564</v>
+      </c>
+      <c r="D86">
+        <v>1.1135999999999999</v>
+      </c>
+      <c r="E86" s="3">
+        <v>45509</v>
+      </c>
+      <c r="F86">
+        <v>1.2343</v>
+      </c>
+      <c r="G86" s="3">
+        <v>45509</v>
+      </c>
+      <c r="H86">
+        <v>1.2285999999999999</v>
+      </c>
+      <c r="I86" t="s">
+        <v>43</v>
+      </c>
+      <c r="J86">
+        <f t="shared" si="1"/>
+        <v>5.7000000000000384</v>
+      </c>
+      <c r="K86">
+        <f t="shared" si="0"/>
+        <v>10.106382978723474</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>45505</v>
+      </c>
+      <c r="B87">
+        <v>9.5</v>
+      </c>
+      <c r="C87">
+        <v>562</v>
+      </c>
+      <c r="D87">
+        <v>1.1169</v>
+      </c>
+      <c r="E87" s="3">
+        <v>45509</v>
+      </c>
+      <c r="F87">
+        <v>1.2406999999999999</v>
+      </c>
+      <c r="G87" s="3">
+        <v>45509</v>
+      </c>
+      <c r="H87">
+        <v>1.2341</v>
+      </c>
+      <c r="I87" t="s">
+        <v>43</v>
+      </c>
+      <c r="J87">
+        <f t="shared" si="1"/>
+        <v>6.5999999999999392</v>
+      </c>
+      <c r="K87">
+        <f t="shared" si="0"/>
+        <v>11.743772241992774</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
putting things together for Matt
</commit_message>
<xml_diff>
--- a/01_Raw_data/POC.xlsx
+++ b/01_Raw_data/POC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111888A0-A223-47DA-8685-D104FF51624B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BF2BBA7-AB7E-490B-9828-9A162B84C227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -546,22 +546,22 @@
   <dimension ref="A1:K95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O86" sqref="O86"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.40625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
-    <col min="5" max="5" width="13.86328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.86328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -596,7 +596,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>45353</v>
       </c>
@@ -633,7 +633,7 @@
         <v>75.838926174495739</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>45019</v>
       </c>
@@ -670,7 +670,7 @@
         <v>6.6339066339067223</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>45355</v>
       </c>
@@ -707,7 +707,7 @@
         <v>7.326007326007332</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>45355</v>
       </c>
@@ -744,7 +744,7 @@
         <v>8.1936685288639843</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>45376</v>
       </c>
@@ -781,7 +781,7 @@
         <v>9.1726618705033847</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>45376</v>
       </c>
@@ -818,7 +818,7 @@
         <v>7.089552238806017</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>45397</v>
       </c>
@@ -837,7 +837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>45391</v>
       </c>
@@ -856,7 +856,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>45355</v>
       </c>
@@ -893,7 +893,7 @@
         <v>2.2865853658537452</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>45397</v>
       </c>
@@ -930,7 +930,7 @@
         <v>12.315270935960601</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>45385</v>
       </c>
@@ -967,7 +967,7 @@
         <v>0.87124878993235522</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>45391</v>
       </c>
@@ -1004,7 +1004,7 @@
         <v>13.29949238578669</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>45391</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>29.107142857142826</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>45047</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>71.755725190840266</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>45376</v>
       </c>
@@ -1115,7 +1115,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45019</v>
       </c>
@@ -1152,7 +1152,7 @@
         <v>11.627906976744121</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45376</v>
       </c>
@@ -1189,7 +1189,7 @@
         <v>4.4692737430166805</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45376</v>
       </c>
@@ -1226,7 +1226,7 @@
         <v>9.2957746478875514</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44280</v>
       </c>
@@ -1263,7 +1263,7 @@
         <v>13.79962192816609</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45400</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>45.102505694760907</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45400</v>
       </c>
@@ -1337,7 +1337,7 @@
         <v>5.525846702317077</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45355</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>5.9149722735672263</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45355</v>
       </c>
@@ -1411,7 +1411,7 @@
         <v>5.2346570397110153</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45413</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>12.145748987854711</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>45400</v>
       </c>
@@ -1485,7 +1485,7 @@
         <v>6.4864864864861715</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>45047</v>
       </c>
@@ -1522,7 +1522,7 @@
         <v>8.6021505376343566</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>45355</v>
       </c>
@@ -1559,7 +1559,7 @@
         <v>6.126126126126251</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>45355</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>11.460258780036938</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>45376</v>
       </c>
@@ -1633,7 +1633,7 @@
         <v>2.752293577981348</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>45385</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>10.609037328094443</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>45376</v>
       </c>
@@ -1707,7 +1707,7 @@
         <v>5.1282051282049697</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>45376</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>5.6558363417568316</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>45385</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>22.98850574712646</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>45047</v>
       </c>
@@ -1818,7 +1818,7 @@
         <v>4.2521994134899188</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>45355</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>4.676258992806039</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>45355</v>
       </c>
@@ -1892,7 +1892,7 @@
         <v>13.120567375886656</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>45385</v>
       </c>
@@ -1929,7 +1929,7 @@
         <v>-1000.132625994695</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>45355</v>
       </c>
@@ -1966,7 +1966,7 @@
         <v>2.9090909090909922</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>45385</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>45047</v>
       </c>
@@ -2037,7 +2037,7 @@
         <v>34.965034965034221</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>45400</v>
       </c>
@@ -2074,7 +2074,7 @@
         <v>5.7142857142855386</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>45397</v>
       </c>
@@ -2111,7 +2111,7 @@
         <v>74.855491329479236</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>45391</v>
       </c>
@@ -2148,7 +2148,7 @@
         <v>23.317865429234349</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>45391</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>3.231939163497954</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45404</v>
       </c>
@@ -2222,7 +2222,7 @@
         <v>10.958904109589238</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>45406</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>208.39999999999924</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>45025</v>
       </c>
@@ -2296,7 +2296,7 @@
         <v>42.487046632124276</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>45038</v>
       </c>
@@ -2333,7 +2333,7 @@
         <v>65.972222222221902</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>45406</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>15.122873345935741</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>45397</v>
       </c>
@@ -2407,7 +2407,7 @@
         <v>13.130252100840289</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>45397</v>
       </c>
@@ -2444,7 +2444,7 @@
         <v>31.738035264483486</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>45397</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>9.7500000000000355</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>45420</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>8.04828973843059</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>45420</v>
       </c>
@@ -2555,7 +2555,7 @@
         <v>1.6666666666666885</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>45404</v>
       </c>
@@ -2592,7 +2592,7 @@
         <v>8.8631984585740611</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>45420</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>21.448999046711332</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>45404</v>
       </c>
@@ -2666,7 +2666,7 @@
         <v>5.7142857142859302</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>45420</v>
       </c>
@@ -2703,7 +2703,7 @@
         <v>1.9848771266540555</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>45415</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>1.7985611510789385</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>45404</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>2.9978586723767813</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>45415</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>15.845070422535422</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>45413</v>
       </c>
@@ -2851,7 +2851,7 @@
         <v>44.265593561368256</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>45415</v>
       </c>
@@ -2888,7 +2888,7 @@
         <v>5.4669703872436397</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>45420</v>
       </c>
@@ -2925,7 +2925,7 @@
         <v>2.7571580063626042</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>45413</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>82.442748091604145</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>45413</v>
       </c>
@@ -2999,7 +2999,7 @@
         <v>25.306122448979526</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>45413</v>
       </c>
@@ -3036,7 +3036,7 @@
         <v>21.192052980132324</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>45415</v>
       </c>
@@ -3073,7 +3073,7 @@
         <v>5.5555555555558245</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>45484</v>
       </c>
@@ -3110,7 +3110,7 @@
         <v>2.6465028355384606</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>45475</v>
       </c>
@@ -3147,7 +3147,7 @@
         <v>6.0185185185183698</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>45484</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>-0.18181818181816178</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>45442</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>6.1790668348046989</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>45484</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>-1.2433392539967052</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>45475</v>
       </c>
@@ -3295,7 +3295,7 @@
         <v>7.7562326869809857</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2">
         <v>45442</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>3.2258064516127654</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2">
         <v>45442</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>1.7733990147783487</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>45484</v>
       </c>
@@ -3406,7 +3406,7 @@
         <v>6.9029850746269332</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>45484</v>
       </c>
@@ -3443,7 +3443,7 @@
         <v>12.226277372262642</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>45505</v>
       </c>
@@ -3480,7 +3480,7 @@
         <v>12.566371681415726</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>45502</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>15.714285714285568</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>45502</v>
       </c>
@@ -3554,7 +3554,7 @@
         <v>7.992895204262787</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2">
         <v>45502</v>
       </c>
@@ -3591,7 +3591,7 @@
         <v>10.830324909747301</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2">
         <v>45505</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>11.690647482014697</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>45502</v>
       </c>
@@ -3665,7 +3665,7 @@
         <v>6.7495559502664761</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>45502</v>
       </c>
@@ -3702,7 +3702,7 @@
         <v>10.106382978723474</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>45505</v>
       </c>
@@ -3739,7 +3739,7 @@
         <v>11.743772241992774</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>45502</v>
       </c>
@@ -3772,11 +3772,11 @@
         <v>696.99999999999989</v>
       </c>
       <c r="K88">
-        <f t="shared" si="0"/>
+        <f>J88/(C88/1000)</f>
         <v>1240.2135231316722</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>45505</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>45505</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>3.0357142857139512</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2">
         <v>45505</v>
       </c>
@@ -3887,7 +3887,7 @@
         <v>4.4563279857396552</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2">
         <v>45505</v>
       </c>
@@ -3924,7 +3924,7 @@
         <v>3.1627906976744837</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2">
         <v>45505</v>
       </c>
@@ -3961,7 +3961,7 @@
         <v>5.2224371373306084</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2">
         <v>45505</v>
       </c>
@@ -3998,7 +3998,7 @@
         <v>3.4013605442175288</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2">
         <v>45505</v>
       </c>

</xml_diff>

<commit_message>
fixed k600 code and updated poc
</commit_message>
<xml_diff>
--- a/01_Raw_data/POC.xlsx
+++ b/01_Raw_data/POC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A961E6-545B-401F-BB84-8F285D294854}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF41991A-B2BA-408C-ADB3-EA03695D972B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
   <si>
     <t>Sampled</t>
   </si>
@@ -543,11 +543,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099139EA-B059-430C-B410-93782515C830}">
-  <dimension ref="A1:K100"/>
+  <dimension ref="A1:K108"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N114" sqref="N114"/>
+      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H98" sqref="H98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
         <v>11.299999999999866</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K100" si="0">J2/(C2/1000)</f>
+        <f t="shared" ref="K2:K108" si="0">J2/(C2/1000)</f>
         <v>75.838926174495739</v>
       </c>
     </row>
@@ -699,7 +699,7 @@
         <v>15</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J100" si="1">(F4-H4)*1000</f>
+        <f t="shared" ref="J4:J108" si="1">(F4-H4)*1000</f>
         <v>4.0000000000000036</v>
       </c>
       <c r="K4">
@@ -4218,6 +4218,302 @@
       <c r="K100">
         <f t="shared" si="0"/>
         <v>4.2253521126759823</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>45526</v>
+      </c>
+      <c r="B101">
+        <v>5</v>
+      </c>
+      <c r="C101">
+        <v>1060</v>
+      </c>
+      <c r="D101">
+        <v>1.0873999999999999</v>
+      </c>
+      <c r="E101" s="3">
+        <v>45534</v>
+      </c>
+      <c r="F101">
+        <v>1.3194999999999999</v>
+      </c>
+      <c r="G101" s="2">
+        <v>45538</v>
+      </c>
+      <c r="H101">
+        <v>1.3109999999999999</v>
+      </c>
+      <c r="I101" t="s">
+        <v>45</v>
+      </c>
+      <c r="J101">
+        <f t="shared" si="1"/>
+        <v>8.499999999999952</v>
+      </c>
+      <c r="K101">
+        <f t="shared" si="0"/>
+        <v>8.0188679245282568</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>45527</v>
+      </c>
+      <c r="B102">
+        <v>9</v>
+      </c>
+      <c r="C102">
+        <v>556</v>
+      </c>
+      <c r="D102">
+        <v>1.1223000000000001</v>
+      </c>
+      <c r="E102" s="3">
+        <v>45534</v>
+      </c>
+      <c r="F102">
+        <v>1.339</v>
+      </c>
+      <c r="G102" s="2">
+        <v>45538</v>
+      </c>
+      <c r="H102">
+        <v>1.3368</v>
+      </c>
+      <c r="I102" t="s">
+        <v>45</v>
+      </c>
+      <c r="J102">
+        <f t="shared" si="1"/>
+        <v>2.1999999999999797</v>
+      </c>
+      <c r="K102">
+        <f t="shared" si="0"/>
+        <v>3.9568345323740641</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>45527</v>
+      </c>
+      <c r="B103">
+        <v>15</v>
+      </c>
+      <c r="C103">
+        <v>558</v>
+      </c>
+      <c r="D103">
+        <v>1.1051</v>
+      </c>
+      <c r="E103" s="3">
+        <v>45534</v>
+      </c>
+      <c r="F103">
+        <v>1.3209</v>
+      </c>
+      <c r="G103" s="2">
+        <v>45538</v>
+      </c>
+      <c r="H103">
+        <v>1.319</v>
+      </c>
+      <c r="I103" t="s">
+        <v>45</v>
+      </c>
+      <c r="J103">
+        <f t="shared" si="1"/>
+        <v>1.9000000000000128</v>
+      </c>
+      <c r="K103">
+        <f t="shared" si="0"/>
+        <v>3.405017921146976</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>45527</v>
+      </c>
+      <c r="B104">
+        <v>7</v>
+      </c>
+      <c r="C104">
+        <v>559</v>
+      </c>
+      <c r="D104">
+        <v>1.0774999999999999</v>
+      </c>
+      <c r="E104" s="3">
+        <v>45534</v>
+      </c>
+      <c r="F104">
+        <v>1.2995000000000001</v>
+      </c>
+      <c r="G104" s="2">
+        <v>45538</v>
+      </c>
+      <c r="H104">
+        <v>1.2928999999999999</v>
+      </c>
+      <c r="I104" t="s">
+        <v>45</v>
+      </c>
+      <c r="J104">
+        <f t="shared" si="1"/>
+        <v>6.6000000000001613</v>
+      </c>
+      <c r="K104">
+        <f t="shared" si="0"/>
+        <v>11.806797853309769</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A105" s="2">
+        <v>45526</v>
+      </c>
+      <c r="B105" t="s">
+        <v>8</v>
+      </c>
+      <c r="C105">
+        <v>1077</v>
+      </c>
+      <c r="D105">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="E105" s="3">
+        <v>45534</v>
+      </c>
+      <c r="F105">
+        <v>1.3069</v>
+      </c>
+      <c r="G105" s="2">
+        <v>45538</v>
+      </c>
+      <c r="H105">
+        <v>1.2948</v>
+      </c>
+      <c r="I105" t="s">
+        <v>45</v>
+      </c>
+      <c r="J105">
+        <f t="shared" si="1"/>
+        <v>12.1</v>
+      </c>
+      <c r="K105">
+        <f t="shared" si="0"/>
+        <v>11.234911792014856</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>45527</v>
+      </c>
+      <c r="B106" t="s">
+        <v>13</v>
+      </c>
+      <c r="C106">
+        <v>572</v>
+      </c>
+      <c r="D106">
+        <v>1.1362000000000001</v>
+      </c>
+      <c r="E106" s="3">
+        <v>45534</v>
+      </c>
+      <c r="F106">
+        <v>1.3665</v>
+      </c>
+      <c r="G106" s="2">
+        <v>45538</v>
+      </c>
+      <c r="H106">
+        <v>1.3612</v>
+      </c>
+      <c r="I106" t="s">
+        <v>45</v>
+      </c>
+      <c r="J106">
+        <f t="shared" si="1"/>
+        <v>5.3000000000000824</v>
+      </c>
+      <c r="K106">
+        <f t="shared" si="0"/>
+        <v>9.2657342657344106</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>45527</v>
+      </c>
+      <c r="B107">
+        <v>13</v>
+      </c>
+      <c r="C107">
+        <v>559</v>
+      </c>
+      <c r="D107">
+        <v>1.1144000000000001</v>
+      </c>
+      <c r="E107" s="3">
+        <v>45534</v>
+      </c>
+      <c r="F107">
+        <v>1.3347</v>
+      </c>
+      <c r="G107" s="2">
+        <v>45538</v>
+      </c>
+      <c r="H107">
+        <v>1.3326</v>
+      </c>
+      <c r="I107" t="s">
+        <v>45</v>
+      </c>
+      <c r="J107">
+        <f t="shared" si="1"/>
+        <v>2.0999999999999908</v>
+      </c>
+      <c r="K107">
+        <f t="shared" si="0"/>
+        <v>3.7567084078711819</v>
+      </c>
+    </row>
+    <row r="108" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>45527</v>
+      </c>
+      <c r="B108">
+        <v>3</v>
+      </c>
+      <c r="C108">
+        <v>559</v>
+      </c>
+      <c r="D108">
+        <v>1.1178999999999999</v>
+      </c>
+      <c r="E108" s="3">
+        <v>45534</v>
+      </c>
+      <c r="F108">
+        <v>1.3354999999999999</v>
+      </c>
+      <c r="G108" s="2">
+        <v>45538</v>
+      </c>
+      <c r="H108">
+        <v>1.3354999999999999</v>
+      </c>
+      <c r="I108" t="s">
+        <v>45</v>
+      </c>
+      <c r="J108">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K108">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixing stuff to mmol
</commit_message>
<xml_diff>
--- a/01_Raw_data/POC.xlsx
+++ b/01_Raw_data/POC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF41991A-B2BA-408C-ADB3-EA03695D972B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{321DBB71-A84E-4BE4-B741-E8C6FD33E966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15270" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
+    <workbookView xWindow="-24075" yWindow="1125" windowWidth="18900" windowHeight="10965" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="46">
   <si>
     <t>Sampled</t>
   </si>
@@ -543,11 +543,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099139EA-B059-430C-B410-93782515C830}">
-  <dimension ref="A1:K108"/>
+  <dimension ref="A1:K126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A80" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H98" sqref="H98"/>
+      <pane ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I126" sqref="I126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
         <v>11.299999999999866</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K108" si="0">J2/(C2/1000)</f>
+        <f t="shared" ref="K2:K114" si="0">J2/(C2/1000)</f>
         <v>75.838926174495739</v>
       </c>
     </row>
@@ -699,7 +699,7 @@
         <v>15</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J108" si="1">(F4-H4)*1000</f>
+        <f t="shared" ref="J4:J114" si="1">(F4-H4)*1000</f>
         <v>4.0000000000000036</v>
       </c>
       <c r="K4">
@@ -4514,6 +4514,504 @@
       <c r="K108">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B109">
+        <v>13</v>
+      </c>
+      <c r="C109">
+        <v>1078</v>
+      </c>
+      <c r="D109">
+        <v>1.0677000000000001</v>
+      </c>
+      <c r="E109" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F109">
+        <v>1.2854000000000001</v>
+      </c>
+      <c r="G109" s="3">
+        <v>45560</v>
+      </c>
+      <c r="H109">
+        <v>1.2844</v>
+      </c>
+      <c r="I109" t="s">
+        <v>45</v>
+      </c>
+      <c r="J109">
+        <f t="shared" si="1"/>
+        <v>1.0000000000001119</v>
+      </c>
+      <c r="K109">
+        <f t="shared" si="0"/>
+        <v>0.9276437847867457</v>
+      </c>
+    </row>
+    <row r="110" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B110">
+        <v>5</v>
+      </c>
+      <c r="C110">
+        <v>549</v>
+      </c>
+      <c r="D110">
+        <v>1.1220000000000001</v>
+      </c>
+      <c r="E110" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F110">
+        <v>1.3372999999999999</v>
+      </c>
+      <c r="G110" s="3">
+        <v>45560</v>
+      </c>
+      <c r="H110">
+        <v>1.3361000000000001</v>
+      </c>
+      <c r="I110" t="s">
+        <v>45</v>
+      </c>
+      <c r="J110">
+        <f t="shared" si="1"/>
+        <v>1.1999999999998678</v>
+      </c>
+      <c r="K110">
+        <f t="shared" si="0"/>
+        <v>2.185792349726535</v>
+      </c>
+    </row>
+    <row r="111" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B111">
+        <v>15</v>
+      </c>
+      <c r="C111">
+        <v>552</v>
+      </c>
+      <c r="D111">
+        <v>1.1052999999999999</v>
+      </c>
+      <c r="E111" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F111">
+        <v>1.3227</v>
+      </c>
+      <c r="G111" s="3">
+        <v>45560</v>
+      </c>
+      <c r="H111">
+        <v>1.3210999999999999</v>
+      </c>
+      <c r="I111" t="s">
+        <v>45</v>
+      </c>
+      <c r="J111">
+        <f t="shared" si="1"/>
+        <v>1.6000000000000458</v>
+      </c>
+      <c r="K111">
+        <f t="shared" si="0"/>
+        <v>2.8985507246377638</v>
+      </c>
+    </row>
+    <row r="112" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B112" t="s">
+        <v>13</v>
+      </c>
+      <c r="C112">
+        <v>563</v>
+      </c>
+      <c r="D112">
+        <v>1.0768</v>
+      </c>
+      <c r="E112" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F112">
+        <v>1.2930999999999999</v>
+      </c>
+      <c r="G112" s="3">
+        <v>45560</v>
+      </c>
+      <c r="H112">
+        <v>1.2917000000000001</v>
+      </c>
+      <c r="I112" t="s">
+        <v>45</v>
+      </c>
+      <c r="J112">
+        <f t="shared" si="1"/>
+        <v>1.3999999999998458</v>
+      </c>
+      <c r="K112">
+        <f t="shared" si="0"/>
+        <v>2.4866785079926217</v>
+      </c>
+    </row>
+    <row r="113" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A113" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B113">
+        <v>7</v>
+      </c>
+      <c r="C113">
+        <v>556</v>
+      </c>
+      <c r="D113">
+        <v>1.0656000000000001</v>
+      </c>
+      <c r="E113" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F113">
+        <v>1.2803</v>
+      </c>
+      <c r="G113" s="3">
+        <v>45560</v>
+      </c>
+      <c r="H113">
+        <v>1.2802</v>
+      </c>
+      <c r="I113" t="s">
+        <v>45</v>
+      </c>
+      <c r="J113">
+        <f t="shared" si="1"/>
+        <v>9.9999999999988987E-2</v>
+      </c>
+      <c r="K113">
+        <f t="shared" si="0"/>
+        <v>0.17985611510789384</v>
+      </c>
+    </row>
+    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B114">
+        <v>3</v>
+      </c>
+      <c r="C114">
+        <v>564</v>
+      </c>
+      <c r="D114">
+        <v>1.1361000000000001</v>
+      </c>
+      <c r="E114" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F114">
+        <v>1.3529</v>
+      </c>
+      <c r="G114" s="3">
+        <v>45560</v>
+      </c>
+      <c r="H114">
+        <v>1.3519000000000001</v>
+      </c>
+      <c r="I114" t="s">
+        <v>45</v>
+      </c>
+      <c r="J114">
+        <f t="shared" si="1"/>
+        <v>0.99999999999988987</v>
+      </c>
+      <c r="K114">
+        <f t="shared" si="0"/>
+        <v>1.7730496453898759</v>
+      </c>
+    </row>
+    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B115">
+        <v>6</v>
+      </c>
+      <c r="C115">
+        <v>561</v>
+      </c>
+      <c r="D115">
+        <v>2.3589000000000002</v>
+      </c>
+      <c r="E115" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F115">
+        <v>1.3017000000000001</v>
+      </c>
+      <c r="G115" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I115" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B116" t="s">
+        <v>8</v>
+      </c>
+      <c r="C116">
+        <v>560</v>
+      </c>
+      <c r="D116">
+        <v>2.3700999999999999</v>
+      </c>
+      <c r="E116" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F116">
+        <v>1.3005</v>
+      </c>
+      <c r="G116" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I116" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="117" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>45548</v>
+      </c>
+      <c r="B117">
+        <v>9</v>
+      </c>
+      <c r="C117">
+        <v>564</v>
+      </c>
+      <c r="D117">
+        <v>2.323</v>
+      </c>
+      <c r="E117" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F117">
+        <v>1.2911999999999999</v>
+      </c>
+      <c r="G117" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I117" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B118">
+        <v>6.2</v>
+      </c>
+      <c r="C118">
+        <v>535</v>
+      </c>
+      <c r="D118">
+        <v>2.7660999999999998</v>
+      </c>
+      <c r="E118" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F118">
+        <v>1.3334999999999999</v>
+      </c>
+      <c r="G118" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I118" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B119">
+        <v>5.6</v>
+      </c>
+      <c r="C119">
+        <v>541</v>
+      </c>
+      <c r="D119">
+        <v>2.7867999999999999</v>
+      </c>
+      <c r="E119" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F119">
+        <v>12797</v>
+      </c>
+      <c r="G119" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I119" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B120">
+        <v>5.2</v>
+      </c>
+      <c r="C120">
+        <v>545</v>
+      </c>
+      <c r="D120">
+        <v>2.3309000000000002</v>
+      </c>
+      <c r="E120" s="3">
+        <v>45560</v>
+      </c>
+      <c r="F120">
+        <v>1.3212999999999999</v>
+      </c>
+      <c r="G120" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I120" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A121" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B121">
+        <v>9.4</v>
+      </c>
+      <c r="C121">
+        <v>526</v>
+      </c>
+      <c r="D121">
+        <v>2.5398999999999998</v>
+      </c>
+      <c r="E121" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I121" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B122">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="C122">
+        <v>536</v>
+      </c>
+      <c r="D122">
+        <v>2.7149000000000001</v>
+      </c>
+      <c r="E122" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I122" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B123">
+        <v>5.4</v>
+      </c>
+      <c r="C123">
+        <v>546</v>
+      </c>
+      <c r="D123">
+        <v>2.7216</v>
+      </c>
+      <c r="E123" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I123" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B124">
+        <v>3.1</v>
+      </c>
+      <c r="C124">
+        <v>440</v>
+      </c>
+      <c r="D124">
+        <v>2.3492999999999999</v>
+      </c>
+      <c r="E124" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I124" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B125">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C125">
+        <v>424</v>
+      </c>
+      <c r="D125">
+        <v>2.6429</v>
+      </c>
+      <c r="E125" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I125" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>45553</v>
+      </c>
+      <c r="B126">
+        <v>5.3</v>
+      </c>
+      <c r="C126">
+        <v>512</v>
+      </c>
+      <c r="D126">
+        <v>2.694</v>
+      </c>
+      <c r="E126" s="2">
+        <v>45565</v>
+      </c>
+      <c r="I126" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
raw field day data
</commit_message>
<xml_diff>
--- a/01_Raw_data/POC.xlsx
+++ b/01_Raw_data/POC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samanthahowley\Desktop\Howley_Bradford_Streams\01_Raw_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6843C59E-0CE0-4892-BFEE-CE0F2380D958}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4426B2-2602-41D8-9242-652A49077BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="945" windowWidth="18900" windowHeight="10965" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
+    <workbookView xWindow="-24420" yWindow="780" windowWidth="18900" windowHeight="10965" xr2:uid="{E8C412AF-B8A1-4AEE-883E-CEDC17E06380}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -549,8 +549,8 @@
   <dimension ref="A1:K133"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K128" sqref="K128"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K135" sqref="K135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,7 +632,7 @@
         <v>11.299999999999866</v>
       </c>
       <c r="K2">
-        <f t="shared" ref="K2:K126" si="0">J2/(C2/1000)</f>
+        <f t="shared" ref="K2:K132" si="0">J2/(C2/1000)</f>
         <v>75.838926174495739</v>
       </c>
     </row>
@@ -702,7 +702,7 @@
         <v>15</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J126" si="1">(F4-H4)*1000</f>
+        <f t="shared" ref="J4:J132" si="1">(F4-H4)*1000</f>
         <v>4.0000000000000036</v>
       </c>
       <c r="K4">
@@ -5207,8 +5207,19 @@
       <c r="G127" s="2">
         <v>45567</v>
       </c>
+      <c r="H127">
+        <v>1.3001</v>
+      </c>
       <c r="I127" t="s">
         <v>45</v>
+      </c>
+      <c r="J127">
+        <f t="shared" si="1"/>
+        <v>0.29999999999996696</v>
+      </c>
+      <c r="K127">
+        <f t="shared" si="0"/>
+        <v>0.53380782918143577</v>
       </c>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
@@ -5233,11 +5244,22 @@
       <c r="G128" s="2">
         <v>45567</v>
       </c>
+      <c r="H128">
+        <v>1.2985</v>
+      </c>
       <c r="I128" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J128">
+        <f t="shared" si="1"/>
+        <v>0.90000000000012292</v>
+      </c>
+      <c r="K128">
+        <f t="shared" si="0"/>
+        <v>1.7142857142859484</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>46</v>
       </c>
@@ -5259,11 +5281,22 @@
       <c r="G129" s="2">
         <v>45567</v>
       </c>
+      <c r="H129">
+        <v>1.2917000000000001</v>
+      </c>
       <c r="I129" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J129">
+        <f t="shared" si="1"/>
+        <v>0.59999999999993392</v>
+      </c>
+      <c r="K129">
+        <f t="shared" si="0"/>
+        <v>1.1090573012937779</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>46</v>
       </c>
@@ -5285,11 +5318,22 @@
       <c r="G130" s="2">
         <v>45567</v>
       </c>
+      <c r="H130">
+        <v>1.3320000000000001</v>
+      </c>
       <c r="I130" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J130">
+        <f t="shared" si="1"/>
+        <v>3.2999999999998586</v>
+      </c>
+      <c r="K130">
+        <f t="shared" si="0"/>
+        <v>6.0218978102187197</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>46</v>
       </c>
@@ -5311,11 +5355,22 @@
       <c r="G131" s="2">
         <v>45567</v>
       </c>
+      <c r="H131">
+        <v>1.2887</v>
+      </c>
       <c r="I131" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131">
+        <f t="shared" si="1"/>
+        <v>2.9000000000001247</v>
+      </c>
+      <c r="K131">
+        <f t="shared" si="0"/>
+        <v>5.3803339517627542</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>46</v>
       </c>
@@ -5337,11 +5392,22 @@
       <c r="G132" s="2">
         <v>45567</v>
       </c>
+      <c r="H132">
+        <v>1.3153999999999999</v>
+      </c>
       <c r="I132" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132">
+        <f t="shared" si="1"/>
+        <v>0.70000000000014495</v>
+      </c>
+      <c r="K132">
+        <f t="shared" si="0"/>
+        <v>1.2987012987015676</v>
+      </c>
+    </row>
+    <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I133" t="s">
         <v>45</v>
       </c>

</xml_diff>